<commit_message>
Got the target buttons to display. Think I need to refactor the UI  manager before heading further.
</commit_message>
<xml_diff>
--- a/Untitled Turn-based RPG Roguelike/Documents/Damage Formula Calculations.xlsx
+++ b/Untitled Turn-based RPG Roguelike/Documents/Damage Formula Calculations.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\GitHub\Fragment\Untitled Turn-based RPG Roguelike\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BBA5E2-8093-42DF-B16E-7A18B5A52165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C1BFA1-6DDE-450B-AABA-C16374A417BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33750" yWindow="1665" windowWidth="21600" windowHeight="12825" xr2:uid="{EA1E9C1B-0744-4AA4-98CD-91390634F9B9}"/>
+    <workbookView xWindow="6525" yWindow="930" windowWidth="21600" windowHeight="12825" activeTab="1" xr2:uid="{EA1E9C1B-0744-4AA4-98CD-91390634F9B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>Formula</t>
   </si>
@@ -60,6 +61,27 @@
   </si>
   <si>
     <t>Buffer</t>
+  </si>
+  <si>
+    <t>Aggression</t>
+  </si>
+  <si>
+    <t>Discipline</t>
+  </si>
+  <si>
+    <t>Weapon</t>
+  </si>
+  <si>
+    <t>Formula: 2x Aggression</t>
+  </si>
+  <si>
+    <t>Formula: 2x Discipline</t>
+  </si>
+  <si>
+    <t>Skill</t>
+  </si>
+  <si>
+    <t>Formula: +Damage</t>
   </si>
 </sst>
 </file>
@@ -95,8 +117,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -112,6 +138,1708 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$3:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$G$3:$G$22</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>6.3636363636363633</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.833333333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.384615384615385</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.375</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.117647058823529</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.8888888888888888</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.6842105263157894</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.3333333333333335</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.1818181818181817</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.0434782608695654</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.9166666666666665</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.6923076923076925</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.5925925925925926</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.4137931034482758</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.3333333333333335</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-50A6-42C9-8A9A-EA6B3FAAFAA3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$23:$B$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$G$23:$G$42</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>13.636363636363637</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.538461538461538</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.714285714285714</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.375</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.8235294117647065</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.3333333333333339</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.8947368421052628</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.1428571428571432</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.8181818181818183</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.5217391304347823</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.25</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.7692307692307692</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.5555555555555554</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.3571428571428568</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.1724137931034484</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-50A6-42C9-8A9A-EA6B3FAAFAA3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$43:$B$62</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$G$43:$G$62</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>22.727272727272727</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.833333333333332</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19.23076923076923</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17.857142857142858</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.666666666666668</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.625</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14.705882352941176</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13.888888888888889</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13.157894736842104</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.904761904761905</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.363636363636363</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10.869565217391305</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10.416666666666666</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.615384615384615</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9.2592592592592595</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.9285714285714288</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.6206896551724146</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8.3333333333333339</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-50A6-42C9-8A9A-EA6B3FAAFAA3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$63:$B$82</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$G$63:$G$82</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>31.818181818181817</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29.166666666666668</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26.923076923076923</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23.333333333333332</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21.875</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20.588235294117649</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19.444444444444443</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18.421052631578949</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16.666666666666668</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15.909090909090908</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15.217391304347826</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.583333333333334</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>13.461538461538462</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12.962962962962964</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>12.068965517241379</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>11.666666666666666</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-50A6-42C9-8A9A-EA6B3FAAFAA3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$83:$B$102</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$83:$B$102</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$G$83:$G$102</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>40.909090909090907</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>37.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>34.615384615384613</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32.142857142857146</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28.125</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>26.470588235294116</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.684210526315791</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21.428571428571427</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20.454545454545453</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>19.565217391304348</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>18.75</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17.307692307692307</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16.666666666666668</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>16.071428571428573</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>15.517241379310345</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-50A6-42C9-8A9A-EA6B3FAAFAA3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="412325104"/>
+        <c:axId val="274676176"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="412325104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="274676176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="274676176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="412325104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57991F3B-DACC-FA8B-4251-D18D2D6ACE4C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -411,15 +2139,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03E5F6F1-6485-47E8-B9B3-A6443E282EBF}">
-  <dimension ref="A1:J102"/>
+  <dimension ref="A1:N102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B102" sqref="B102"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -438,8 +2166,11 @@
       <c r="J1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="N1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -459,7 +2190,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -482,7 +2213,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -502,7 +2233,7 @@
         <v>1.9047619047619047</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -522,7 +2253,7 @@
         <v>2.8571428571428572</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -542,7 +2273,7 @@
         <v>3.8095238095238093</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -562,7 +2293,7 @@
         <v>4.7619047619047619</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -582,7 +2313,7 @@
         <v>5.7142857142857144</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -602,7 +2333,7 @@
         <v>6.666666666666667</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -622,7 +2353,7 @@
         <v>7.6190476190476186</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -642,7 +2373,7 @@
         <v>8.5714285714285712</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -662,7 +2393,7 @@
         <v>9.5238095238095237</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -682,7 +2413,7 @@
         <v>10.476190476190476</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -702,7 +2433,7 @@
         <v>11.428571428571429</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -722,7 +2453,7 @@
         <v>12.380952380952381</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2465,4 +4196,2470 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{711FC013-14B4-445C-95C1-05FA2C2DE02A}">
+  <dimension ref="A1:H102"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <f>A3*2</f>
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <f>B3*2</f>
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <f>C3+$F$3</f>
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3" s="2">
+        <f>E3*$H$3/($H$3+D3)</f>
+        <v>6.3636363636363633</v>
+      </c>
+      <c r="H3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C67" si="0">A4*2</f>
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D67" si="1">B4*2</f>
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E67" si="2">C4+$F$3</f>
+        <v>7</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" ref="G4:G67" si="3">E4*$H$3/($H$3+D4)</f>
+        <v>5.833333333333333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="3"/>
+        <v>5.384615384615385</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="3"/>
+        <v>4.666666666666667</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="3"/>
+        <v>4.375</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="3"/>
+        <v>4.117647058823529</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="3"/>
+        <v>3.8888888888888888</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="3"/>
+        <v>3.6842105263157894</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="3"/>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="3"/>
+        <v>3.3333333333333335</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="3"/>
+        <v>3.1818181818181817</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="3"/>
+        <v>3.0434782608695654</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" si="3"/>
+        <v>2.9166666666666665</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" si="3"/>
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" si="3"/>
+        <v>2.6923076923076925</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>17</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="G19" s="2">
+        <f t="shared" si="3"/>
+        <v>2.5925925925925926</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" si="3"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>19</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" si="3"/>
+        <v>2.4137931034482758</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="G22" s="2">
+        <f t="shared" si="3"/>
+        <v>2.3333333333333335</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="3"/>
+        <v>13.636363636363637</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="3"/>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="3"/>
+        <v>11.538461538461538</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="3"/>
+        <v>10.714285714285714</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>5</v>
+      </c>
+      <c r="B27">
+        <v>5</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>5</v>
+      </c>
+      <c r="B28">
+        <v>6</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="3"/>
+        <v>9.375</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>7</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="3"/>
+        <v>8.8235294117647065</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <v>8</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="G30" s="2">
+        <f t="shared" si="3"/>
+        <v>8.3333333333333339</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>5</v>
+      </c>
+      <c r="B31">
+        <v>9</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="3"/>
+        <v>7.8947368421052628</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="B32">
+        <v>10</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="G32" s="2">
+        <f t="shared" si="3"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>5</v>
+      </c>
+      <c r="B33">
+        <v>11</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="G33" s="2">
+        <f t="shared" si="3"/>
+        <v>7.1428571428571432</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>5</v>
+      </c>
+      <c r="B34">
+        <v>12</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="G34" s="2">
+        <f t="shared" si="3"/>
+        <v>6.8181818181818183</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>5</v>
+      </c>
+      <c r="B35">
+        <v>13</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="G35" s="2">
+        <f t="shared" si="3"/>
+        <v>6.5217391304347823</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>5</v>
+      </c>
+      <c r="B36">
+        <v>14</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="G36" s="2">
+        <f t="shared" si="3"/>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>5</v>
+      </c>
+      <c r="B37">
+        <v>15</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="G37" s="2">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>5</v>
+      </c>
+      <c r="B38">
+        <v>16</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="G38" s="2">
+        <f t="shared" si="3"/>
+        <v>5.7692307692307692</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>5</v>
+      </c>
+      <c r="B39">
+        <v>17</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="G39" s="2">
+        <f t="shared" si="3"/>
+        <v>5.5555555555555554</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>5</v>
+      </c>
+      <c r="B40">
+        <v>18</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="G40" s="2">
+        <f t="shared" si="3"/>
+        <v>5.3571428571428568</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>5</v>
+      </c>
+      <c r="B41">
+        <v>19</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="G41" s="2">
+        <f t="shared" si="3"/>
+        <v>5.1724137931034484</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>5</v>
+      </c>
+      <c r="B42">
+        <v>20</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="G42" s="2">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>10</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="G43" s="2">
+        <f t="shared" si="3"/>
+        <v>22.727272727272727</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>10</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="G44" s="2">
+        <f t="shared" si="3"/>
+        <v>20.833333333333332</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>10</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="G45" s="2">
+        <f t="shared" si="3"/>
+        <v>19.23076923076923</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>10</v>
+      </c>
+      <c r="B46">
+        <v>4</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="G46" s="2">
+        <f t="shared" si="3"/>
+        <v>17.857142857142858</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>10</v>
+      </c>
+      <c r="B47">
+        <v>5</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="G47" s="2">
+        <f t="shared" si="3"/>
+        <v>16.666666666666668</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>10</v>
+      </c>
+      <c r="B48">
+        <v>6</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="G48" s="2">
+        <f t="shared" si="3"/>
+        <v>15.625</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>10</v>
+      </c>
+      <c r="B49">
+        <v>7</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="G49" s="2">
+        <f t="shared" si="3"/>
+        <v>14.705882352941176</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>10</v>
+      </c>
+      <c r="B50">
+        <v>8</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="G50" s="2">
+        <f t="shared" si="3"/>
+        <v>13.888888888888889</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>10</v>
+      </c>
+      <c r="B51">
+        <v>9</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="G51" s="2">
+        <f t="shared" si="3"/>
+        <v>13.157894736842104</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>10</v>
+      </c>
+      <c r="B52">
+        <v>10</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="G52" s="2">
+        <f t="shared" si="3"/>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>10</v>
+      </c>
+      <c r="B53">
+        <v>11</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="G53" s="2">
+        <f t="shared" si="3"/>
+        <v>11.904761904761905</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>10</v>
+      </c>
+      <c r="B54">
+        <v>12</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="G54" s="2">
+        <f t="shared" si="3"/>
+        <v>11.363636363636363</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>10</v>
+      </c>
+      <c r="B55">
+        <v>13</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="G55" s="2">
+        <f t="shared" si="3"/>
+        <v>10.869565217391305</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>10</v>
+      </c>
+      <c r="B56">
+        <v>14</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="G56" s="2">
+        <f t="shared" si="3"/>
+        <v>10.416666666666666</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>10</v>
+      </c>
+      <c r="B57">
+        <v>15</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="G57" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>10</v>
+      </c>
+      <c r="B58">
+        <v>16</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="G58" s="2">
+        <f t="shared" si="3"/>
+        <v>9.615384615384615</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>10</v>
+      </c>
+      <c r="B59">
+        <v>17</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="G59" s="2">
+        <f t="shared" si="3"/>
+        <v>9.2592592592592595</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>10</v>
+      </c>
+      <c r="B60">
+        <v>18</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="G60" s="2">
+        <f t="shared" si="3"/>
+        <v>8.9285714285714288</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>10</v>
+      </c>
+      <c r="B61">
+        <v>19</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="G61" s="2">
+        <f t="shared" si="3"/>
+        <v>8.6206896551724146</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>10</v>
+      </c>
+      <c r="B62">
+        <v>20</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="G62" s="2">
+        <f t="shared" si="3"/>
+        <v>8.3333333333333339</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>15</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="G63" s="2">
+        <f t="shared" si="3"/>
+        <v>31.818181818181817</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>15</v>
+      </c>
+      <c r="B64">
+        <v>2</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="G64" s="2">
+        <f t="shared" si="3"/>
+        <v>29.166666666666668</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>15</v>
+      </c>
+      <c r="B65">
+        <v>3</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="G65" s="2">
+        <f t="shared" si="3"/>
+        <v>26.923076923076923</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>15</v>
+      </c>
+      <c r="B66">
+        <v>4</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="E66">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="G66" s="2">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>15</v>
+      </c>
+      <c r="B67">
+        <v>5</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="E67">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="G67" s="2">
+        <f t="shared" si="3"/>
+        <v>23.333333333333332</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>15</v>
+      </c>
+      <c r="B68">
+        <v>6</v>
+      </c>
+      <c r="C68">
+        <f t="shared" ref="C68:C102" si="4">A68*2</f>
+        <v>30</v>
+      </c>
+      <c r="D68">
+        <f t="shared" ref="D68:D102" si="5">B68*2</f>
+        <v>12</v>
+      </c>
+      <c r="E68">
+        <f t="shared" ref="E68:E102" si="6">C68+$F$3</f>
+        <v>35</v>
+      </c>
+      <c r="G68" s="2">
+        <f t="shared" ref="G68:G102" si="7">E68*$H$3/($H$3+D68)</f>
+        <v>21.875</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>15</v>
+      </c>
+      <c r="B69">
+        <v>7</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="6"/>
+        <v>35</v>
+      </c>
+      <c r="G69" s="2">
+        <f t="shared" si="7"/>
+        <v>20.588235294117649</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>15</v>
+      </c>
+      <c r="B70">
+        <v>8</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="6"/>
+        <v>35</v>
+      </c>
+      <c r="G70" s="2">
+        <f t="shared" si="7"/>
+        <v>19.444444444444443</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>15</v>
+      </c>
+      <c r="B71">
+        <v>9</v>
+      </c>
+      <c r="C71">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="6"/>
+        <v>35</v>
+      </c>
+      <c r="G71" s="2">
+        <f t="shared" si="7"/>
+        <v>18.421052631578949</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>15</v>
+      </c>
+      <c r="B72">
+        <v>10</v>
+      </c>
+      <c r="C72">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="6"/>
+        <v>35</v>
+      </c>
+      <c r="G72" s="2">
+        <f t="shared" si="7"/>
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>15</v>
+      </c>
+      <c r="B73">
+        <v>11</v>
+      </c>
+      <c r="C73">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="6"/>
+        <v>35</v>
+      </c>
+      <c r="G73" s="2">
+        <f t="shared" si="7"/>
+        <v>16.666666666666668</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>15</v>
+      </c>
+      <c r="B74">
+        <v>12</v>
+      </c>
+      <c r="C74">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="6"/>
+        <v>35</v>
+      </c>
+      <c r="G74" s="2">
+        <f t="shared" si="7"/>
+        <v>15.909090909090908</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>15</v>
+      </c>
+      <c r="B75">
+        <v>13</v>
+      </c>
+      <c r="C75">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="5"/>
+        <v>26</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="6"/>
+        <v>35</v>
+      </c>
+      <c r="G75" s="2">
+        <f t="shared" si="7"/>
+        <v>15.217391304347826</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>15</v>
+      </c>
+      <c r="B76">
+        <v>14</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="5"/>
+        <v>28</v>
+      </c>
+      <c r="E76">
+        <f t="shared" si="6"/>
+        <v>35</v>
+      </c>
+      <c r="G76" s="2">
+        <f t="shared" si="7"/>
+        <v>14.583333333333334</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>15</v>
+      </c>
+      <c r="B77">
+        <v>15</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="E77">
+        <f t="shared" si="6"/>
+        <v>35</v>
+      </c>
+      <c r="G77" s="2">
+        <f t="shared" si="7"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>15</v>
+      </c>
+      <c r="B78">
+        <v>16</v>
+      </c>
+      <c r="C78">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="5"/>
+        <v>32</v>
+      </c>
+      <c r="E78">
+        <f t="shared" si="6"/>
+        <v>35</v>
+      </c>
+      <c r="G78" s="2">
+        <f t="shared" si="7"/>
+        <v>13.461538461538462</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>15</v>
+      </c>
+      <c r="B79">
+        <v>17</v>
+      </c>
+      <c r="C79">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="5"/>
+        <v>34</v>
+      </c>
+      <c r="E79">
+        <f t="shared" si="6"/>
+        <v>35</v>
+      </c>
+      <c r="G79" s="2">
+        <f t="shared" si="7"/>
+        <v>12.962962962962964</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>15</v>
+      </c>
+      <c r="B80">
+        <v>18</v>
+      </c>
+      <c r="C80">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="D80">
+        <f t="shared" si="5"/>
+        <v>36</v>
+      </c>
+      <c r="E80">
+        <f t="shared" si="6"/>
+        <v>35</v>
+      </c>
+      <c r="G80" s="2">
+        <f t="shared" si="7"/>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>15</v>
+      </c>
+      <c r="B81">
+        <v>19</v>
+      </c>
+      <c r="C81">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="D81">
+        <f t="shared" si="5"/>
+        <v>38</v>
+      </c>
+      <c r="E81">
+        <f t="shared" si="6"/>
+        <v>35</v>
+      </c>
+      <c r="G81" s="2">
+        <f t="shared" si="7"/>
+        <v>12.068965517241379</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>15</v>
+      </c>
+      <c r="B82">
+        <v>20</v>
+      </c>
+      <c r="C82">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+      <c r="E82">
+        <f t="shared" si="6"/>
+        <v>35</v>
+      </c>
+      <c r="G82" s="2">
+        <f t="shared" si="7"/>
+        <v>11.666666666666666</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>20</v>
+      </c>
+      <c r="B83">
+        <v>1</v>
+      </c>
+      <c r="C83">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="D83">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="E83">
+        <f t="shared" si="6"/>
+        <v>45</v>
+      </c>
+      <c r="G83" s="2">
+        <f t="shared" si="7"/>
+        <v>40.909090909090907</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>20</v>
+      </c>
+      <c r="B84">
+        <v>2</v>
+      </c>
+      <c r="C84">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="D84">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="E84">
+        <f t="shared" si="6"/>
+        <v>45</v>
+      </c>
+      <c r="G84" s="2">
+        <f t="shared" si="7"/>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>20</v>
+      </c>
+      <c r="B85">
+        <v>3</v>
+      </c>
+      <c r="C85">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="D85">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="E85">
+        <f t="shared" si="6"/>
+        <v>45</v>
+      </c>
+      <c r="G85" s="2">
+        <f t="shared" si="7"/>
+        <v>34.615384615384613</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>20</v>
+      </c>
+      <c r="B86">
+        <v>4</v>
+      </c>
+      <c r="C86">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="D86">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="E86">
+        <f t="shared" si="6"/>
+        <v>45</v>
+      </c>
+      <c r="G86" s="2">
+        <f t="shared" si="7"/>
+        <v>32.142857142857146</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>20</v>
+      </c>
+      <c r="B87">
+        <v>5</v>
+      </c>
+      <c r="C87">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="D87">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="E87">
+        <f t="shared" si="6"/>
+        <v>45</v>
+      </c>
+      <c r="G87" s="2">
+        <f t="shared" si="7"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>20</v>
+      </c>
+      <c r="B88">
+        <v>6</v>
+      </c>
+      <c r="C88">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="D88">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="E88">
+        <f t="shared" si="6"/>
+        <v>45</v>
+      </c>
+      <c r="G88" s="2">
+        <f t="shared" si="7"/>
+        <v>28.125</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>20</v>
+      </c>
+      <c r="B89">
+        <v>7</v>
+      </c>
+      <c r="C89">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="D89">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="E89">
+        <f t="shared" si="6"/>
+        <v>45</v>
+      </c>
+      <c r="G89" s="2">
+        <f t="shared" si="7"/>
+        <v>26.470588235294116</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>20</v>
+      </c>
+      <c r="B90">
+        <v>8</v>
+      </c>
+      <c r="C90">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="D90">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="E90">
+        <f t="shared" si="6"/>
+        <v>45</v>
+      </c>
+      <c r="G90" s="2">
+        <f t="shared" si="7"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>20</v>
+      </c>
+      <c r="B91">
+        <v>9</v>
+      </c>
+      <c r="C91">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="D91">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="E91">
+        <f t="shared" si="6"/>
+        <v>45</v>
+      </c>
+      <c r="G91" s="2">
+        <f t="shared" si="7"/>
+        <v>23.684210526315791</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>20</v>
+      </c>
+      <c r="B92">
+        <v>10</v>
+      </c>
+      <c r="C92">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="D92">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="E92">
+        <f t="shared" si="6"/>
+        <v>45</v>
+      </c>
+      <c r="G92" s="2">
+        <f t="shared" si="7"/>
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>20</v>
+      </c>
+      <c r="B93">
+        <v>11</v>
+      </c>
+      <c r="C93">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="D93">
+        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
+      <c r="E93">
+        <f t="shared" si="6"/>
+        <v>45</v>
+      </c>
+      <c r="G93" s="2">
+        <f t="shared" si="7"/>
+        <v>21.428571428571427</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>20</v>
+      </c>
+      <c r="B94">
+        <v>12</v>
+      </c>
+      <c r="C94">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="D94">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+      <c r="E94">
+        <f t="shared" si="6"/>
+        <v>45</v>
+      </c>
+      <c r="G94" s="2">
+        <f t="shared" si="7"/>
+        <v>20.454545454545453</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>20</v>
+      </c>
+      <c r="B95">
+        <v>13</v>
+      </c>
+      <c r="C95">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="D95">
+        <f t="shared" si="5"/>
+        <v>26</v>
+      </c>
+      <c r="E95">
+        <f t="shared" si="6"/>
+        <v>45</v>
+      </c>
+      <c r="G95" s="2">
+        <f t="shared" si="7"/>
+        <v>19.565217391304348</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>20</v>
+      </c>
+      <c r="B96">
+        <v>14</v>
+      </c>
+      <c r="C96">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="D96">
+        <f t="shared" si="5"/>
+        <v>28</v>
+      </c>
+      <c r="E96">
+        <f t="shared" si="6"/>
+        <v>45</v>
+      </c>
+      <c r="G96" s="2">
+        <f t="shared" si="7"/>
+        <v>18.75</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>20</v>
+      </c>
+      <c r="B97">
+        <v>15</v>
+      </c>
+      <c r="C97">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="D97">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="E97">
+        <f t="shared" si="6"/>
+        <v>45</v>
+      </c>
+      <c r="G97" s="2">
+        <f t="shared" si="7"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>20</v>
+      </c>
+      <c r="B98">
+        <v>16</v>
+      </c>
+      <c r="C98">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="D98">
+        <f t="shared" si="5"/>
+        <v>32</v>
+      </c>
+      <c r="E98">
+        <f t="shared" si="6"/>
+        <v>45</v>
+      </c>
+      <c r="G98" s="2">
+        <f t="shared" si="7"/>
+        <v>17.307692307692307</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>20</v>
+      </c>
+      <c r="B99">
+        <v>17</v>
+      </c>
+      <c r="C99">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="D99">
+        <f t="shared" si="5"/>
+        <v>34</v>
+      </c>
+      <c r="E99">
+        <f t="shared" si="6"/>
+        <v>45</v>
+      </c>
+      <c r="G99" s="2">
+        <f t="shared" si="7"/>
+        <v>16.666666666666668</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>20</v>
+      </c>
+      <c r="B100">
+        <v>18</v>
+      </c>
+      <c r="C100">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="D100">
+        <f t="shared" si="5"/>
+        <v>36</v>
+      </c>
+      <c r="E100">
+        <f t="shared" si="6"/>
+        <v>45</v>
+      </c>
+      <c r="G100" s="2">
+        <f t="shared" si="7"/>
+        <v>16.071428571428573</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>20</v>
+      </c>
+      <c r="B101">
+        <v>19</v>
+      </c>
+      <c r="C101">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="D101">
+        <f t="shared" si="5"/>
+        <v>38</v>
+      </c>
+      <c r="E101">
+        <f t="shared" si="6"/>
+        <v>45</v>
+      </c>
+      <c r="G101" s="2">
+        <f t="shared" si="7"/>
+        <v>15.517241379310345</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>20</v>
+      </c>
+      <c r="B102">
+        <v>20</v>
+      </c>
+      <c r="C102">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="D102">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+      <c r="E102">
+        <f t="shared" si="6"/>
+        <v>45</v>
+      </c>
+      <c r="G102" s="2">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>